<commit_message>
corrección final parte 2
</commit_message>
<xml_diff>
--- a/TP1/noticias.xlsx
+++ b/TP1/noticias.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A122"/>
+  <dimension ref="A1:A121"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,7 +441,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/el-mundo/edmundo-gonzalez-urrutia-llego-a-espana-que-le-otorgo-asilo-politico-nid08092024/</t>
+          <t>https://www.lanacion.com.ar/el-mundo/asi-fue-la-salida-de-edmundo-gonzalez-de-venezuela-amenazado-por-la-dictadura-de-nicolas-maduro-nid08092024/</t>
         </is>
       </c>
     </row>
@@ -455,14 +455,14 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/el-mundo/maria-corina-machado-resiste-el-hostigamiento-edmundo-luchara-desde-afuera-y-volvera-para-asumir-la-nid08092024/</t>
+          <t>https://www.lanacion.com.ar/opinion/la-casta-que-rodea-al-presidente-nid08092024/</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/opinion/la-casta-que-rodea-al-presidente-nid08092024/</t>
+          <t>https://www.lanacion.com.ar/deportes/tenis/jannik-sinner-campeon-del-us-open-el-italiano-vencio-a-taylor-fritz-y-se-encumbro-tras-el-ruido-que-nid08092024/</t>
         </is>
       </c>
     </row>
@@ -476,42 +476,42 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/el-mundo/oriente-medio-un-argentino-fue-asesinado-en-un-ataque-terrorista-donde-murieron-otros-dos-civiles-nid08092024/</t>
+          <t>https://www.lanacion.com.ar/deportes/tenis/jannik-sinner-campeon-del-us-open-el-italiano-vencio-a-taylor-fritz-y-se-encumbro-tras-el-ruido-que-nid08092024/</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/el-mundo/asi-fue-la-salida-de-edmundo-gonzalez-de-venezuela-amenazado-por-la-dictadura-de-nicolas-maduro-nid08092024/</t>
+          <t>https://www.lanacion.com.ar/el-mundo/desde-espana-edmundo-gonzalez-urrutia-denuncio-presiones-coacciones-y-amenazas-para-impedir-su-nid08092024/</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/el-mundo/colombia-o-argentina-inteligencia-artificial-predice-resultado-del-esperado-partido-nid08092024/</t>
+          <t>https://www.lanacion.com.ar/politica/bandera-roja-y-martillo-la-justicia-ordeno-retomar-los-remates-de-bienes-de-lazaro-baez-nid08092024/</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/el-mundo/el-hijo-del-argentino-asesinado-en-cisjordania-es-un-sobreviviente-al-ataque-de-hamas-papa-me-nid08092024/</t>
+          <t>https://www.lanacion.com.ar/estados-unidos/donald-trump-amenaza-con-encarcelar-a-quienes-cometieron-fraude-electoral-en-2020-nid08092024/</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/deportes/futbol/el-golazo-de-chilena-de-dinamarca-en-la-victoria-ante-serbia-por-la-nations-league-la-pirueta-de-nid08092024/</t>
+          <t>https://www.lanacion.com.ar/sociedad/cortina-de-humo-que-es-el-fenomeno-que-llegara-a-buenos-aires-este-lunes-y-que-fue-advertido-por-el-nid08092024/</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/el-mundo/oriente-medio-un-argentino-fue-asesinado-en-un-ataque-terrorista-donde-murieron-otros-dos-civiles-nid08092024/</t>
+          <t>https://www.lanacion.com.ar/sociedad/cortina-de-humo-que-es-el-fenomeno-que-llegara-a-buenos-aires-este-lunes-y-que-fue-advertido-por-el-nid08092024/</t>
         </is>
       </c>
     </row>
@@ -525,112 +525,112 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/sociedad/cortina-de-humo-que-es-el-fenomeno-que-llegara-a-buenos-aires-este-lunes-y-que-fue-advertido-por-el-nid08092024/</t>
+          <t>https://www.lanacion.com.ar/el-mundo/el-hijo-del-argentino-asesinado-en-cisjordania-es-un-sobreviviente-al-ataque-de-hamas-papa-me-nid08092024/</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/seguridad/adn-del-crimen-confirman-la-condena-para-el-poderoso-juez-que-era-la-pieza-clave-de-la-banda-formada-nid08092024/</t>
+          <t>https://www.lanacion.com.ar/autos/al-volante/grave-denuncia-del-arbitro-andres-merlos-contra-el-presidente-de-talleres-tras-el-partido-con-boca-nid08092024/</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/politica/el-pacto-no-escrito-entre-javier-milei-y-cristina-kirchner-nid07092024/</t>
+          <t>https://www.lanacion.com.ar/el-mundo/maria-corina-machado-resiste-el-hostigamiento-edmundo-luchara-desde-afuera-y-volvera-para-asumir-la-nid08092024/</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/el-mundo/el-hijo-del-argentino-asesinado-en-cisjordania-es-un-sobreviviente-al-ataque-de-hamas-papa-me-nid08092024/</t>
+          <t>https://www.lanacion.com.ar/politica/militancia-partidaria-y-extorsion-de-los-sindicatos-pro-va-por-la-privatizacion-de-aerolineas-nid08092024/</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/sociedad/monociclos-electricos-las-razones-por-las-que-se-extiende-su-uso-y-claves-sobre-la-legislacion-que-nid08092024/</t>
+          <t>https://www.lanacion.com.ar/politica/los-diplomaticos-van-al-paro-y-apuntan-a-mondino-por-el-pago-de-ganancias-nid08092024/</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/deportes/futbol/el-golazo-de-chilena-de-dinamarca-en-la-victoria-ante-serbia-por-la-nations-league-la-pirueta-de-nid08092024/</t>
+          <t>https://www.lanacion.com.ar/sociedad/puerta-a-puerta-asi-es-el-operativo-en-6947-domicilios-para-conocer-cuantos-portenos-ya-tuvieron-nid08092024/</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/economia/para-que-importar-para-poder-exportar-nid08092024/</t>
+          <t>https://www.lanacion.com.ar/politica/bandera-roja-y-martillo-la-justicia-ordeno-retomar-los-remates-de-bienes-de-lazaro-baez-nid08092024/</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/seguridad/una-turista-italiana-denuncio-que-fue-agredida-sexualmente-en-los-esteros-del-ibera-nid08092024/</t>
+          <t>https://www.lanacion.com.ar/el-mundo/un-patrullero-atropello-a-tres-personas-durante-una-persecucion-en-un-exclusivo-barrio-de-madrid-nid08092024/</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/deportes/atletismo/el-increible-accidente-de-la-paratleta-italiana-que-perdio-la-medalla-dorada-y-conmovio-a-todos-en-nid08092024/</t>
+          <t>https://www.lanacion.com.ar/economia/para-que-importar-para-poder-exportar-nid08092024/</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/sociedad/me-enseno-a-posicionar-mi-negocio-el-fuerte-impacto-de-un-programa-educativo-gratuito-y-con-nid08092024/</t>
+          <t>https://www.lanacion.com.ar/seguridad/asesinaron-a-una-sargento-de-la-policia-bonaerense-mientras-trabajaba-como-chofer-de-una-app-nid08092024/</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/economia/campo/el-padre-guillermo-furlong-rescato-las-observaciones-de-charles-darwin-sobre-los-gauchos-argentinos-nid18052024/</t>
+          <t>https://www.lanacion.com.ar/seguridad/adn-del-crimen-confirman-la-condena-para-el-poderoso-juez-que-era-la-pieza-clave-de-la-banda-formada-nid08092024/</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/seguridad/un-policia-murio-tras-recibir-una-patada-en-la-espalda-cuando-vecinos-defendieron-a-un-delincuente-nid07092024/</t>
+          <t>https://www.lanacion.com.ar/sociedad/revelador-estudio-uno-de-cada-cuatro-pacientes-en-coma-sigue-teniendo-algun-tipo-de-consciencia-nid08092024/</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/deportes/futbol/fuerte-discusion-entre-el-presidente-de-talleres-y-andres-merlos-ingreso-al-vestuario-con-armas-nid08092024/</t>
+          <t>https://www.lanacion.com.ar/sociedad/me-enseno-a-posicionar-mi-negocio-el-fuerte-impacto-de-un-programa-educativo-gratuito-y-con-nid08092024/</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/economia/las-contradicciones-del-gobierno-juegan-en-contra-de-bajar-el-riesgo-pais-nid08092024/</t>
+          <t>https://www.lanacion.com.ar/el-mundo/colombia-o-argentina-inteligencia-artificial-predice-resultado-del-esperado-partido-nid08092024/</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/deportes/rugby/julian-montoya-tuvo-su-tarde-sonada-el-capitan-llego-a-su-partido-100-en-los-pumas-nid08092024/</t>
+          <t>https://www.lanacion.com.ar/deportes/futbol/river-volvio-a-ganarle-a-boca-en-reserva-y-disfruta-de-un-ano-perfecto-en-el-superclasico-nid08092024/</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/deportes/futbol/un-ataque-de-locura-el-poder-de-fuego-de-la-seleccion-argentina-va-mas-alla-de-messi-y-scaloni-lo-nid08092024/</t>
+          <t>https://www.lanacion.com.ar/deportes/futbol/el-golazo-de-chilena-de-dinamarca-en-la-victoria-ante-serbia-por-la-nations-league-la-pirueta-de-nid08092024/</t>
         </is>
       </c>
     </row>
@@ -644,280 +644,280 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/espectaculos/personajes/pacho-odonnell-el-edadismo-su-adiccion-a-la-gimnasia-su-regreso-a-los-escenarios-y-por-que-hay-que-nid08092024/</t>
+          <t>https://www.lanacion.com.ar/el-mundo/la-larga-lista-de-opositores-perseguidos-que-sufren-el-exilio-impuesto-por-hugo-chavez-y-nicolas-nid08092024/</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/conversaciones-de-domingo/dante-sica-el-programa-de-desregulaciones-de-milei-es-similar-al-de-macri-pero-macri-fue-un-liberal-nid08092024/</t>
+          <t>https://www.lanacion.com.ar/el-mundo/desde-espana-edmundo-gonzalez-urrutia-denuncio-presiones-coacciones-y-amenazas-para-impedir-su-nid08092024/</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/deportes/futbol/la-jugada-del-arquero-de-penarol-que-desato-un-escandalo-tres-expulsados-y-seis-amonestados-nid08092024/</t>
+          <t>https://www.lanacion.com.ar/estados-unidos/donald-trump-amenaza-con-encarcelar-a-quienes-cometieron-fraude-electoral-en-2020-nid08092024/</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/deportes/dibu-martinez-mostro-lo-que-come-el-plantel-de-la-seleccion-argentina-y-sorprendio-a-todos-que-me-nid08092024/</t>
+          <t>https://www.lanacion.com.ar/seguridad/una-turista-italiana-denuncio-que-fue-agredida-sexualmente-en-los-esteros-del-ibera-nid08092024/</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/lifestyle/hija-de-una-argentina-la-foto-que-delato-la-relacion-entre-el-principe-felipe-e-isabel-sartorius-el-nid06092024/</t>
+          <t>https://www.lanacion.com.ar/economia/las-contradicciones-del-gobierno-juegan-en-contra-de-bajar-el-riesgo-pais-nid08092024/</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/economia/martinez-sosa-cobro-comisiones-de-200-mil-polizas-optativas-con-una-trampa-en-gendarmeria-nid08092024/</t>
+          <t>https://www.lanacion.com.ar/seguridad/un-policia-murio-tras-recibir-una-patada-en-la-espalda-cuando-vecinos-defendieron-a-un-delincuente-nid07092024/</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/propiedades/inversiones/la-zona-impensada-en-donde-los-alquileres-dejan-la-renta-mas-alta-del-mercado-10-en-dolares-nid28082024/</t>
+          <t>https://www.lanacion.com.ar/espectaculos/personajes/pacho-odonnell-el-edadismo-su-adiccion-a-la-gimnasia-su-regreso-a-los-escenarios-y-por-que-hay-que-nid08092024/</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/autos/al-volante/los-autos-con-motores-turbo-chicos-siguen-creciendo-que-modelos-los-ofrecen-y-por-que-nid08092024/</t>
+          <t>https://www.lanacion.com.ar/deportes/futbol/la-jugada-del-arquero-de-penarol-que-desato-un-escandalo-tres-expulsados-y-seis-amonestados-nid08092024/</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/espectaculos/musica/waldo-de-los-rios-el-genio-musical-que-cumpliria-90-anos-sus-frustraciones-un-auto-incendiado-y-el-nid07092024/</t>
+          <t>https://www.lanacion.com.ar/economia/martinez-sosa-cobro-comisiones-de-200-mil-polizas-optativas-con-una-trampa-en-gendarmeria-nid08092024/</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/el-mundo/el-papa-cumplio-su-promesa-de-visitar-a-misioneros-argentinos-que-trabajan-en-la-periferia-de-la-nid08092024/</t>
+          <t>https://www.lanacion.com.ar/propiedades/inversiones/la-zona-impensada-en-donde-los-alquileres-dejan-la-renta-mas-alta-del-mercado-10-en-dolares-nid28082024/</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/politica/quien-es-el-agente-inmobiliario-y-principal-sospechoso-de-enviar-un-paquete-explosivo-a-nicolas-pino-nid07092024/</t>
+          <t>https://www.lanacion.com.ar/autos/al-volante/los-autos-con-motores-turbo-chicos-siguen-creciendo-que-modelos-los-ofrecen-y-por-que-nid08092024/</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/tecnologia/kathleen-booth-la-precursora-de-las-redes-neuronales-que-hace-casi-80-anos-nos-enseno-a-hablar-con-nid08092024/</t>
+          <t>https://www.lanacion.com.ar/espectaculos/musica/waldo-de-los-rios-el-genio-musical-que-cumpliria-90-anos-sus-frustraciones-un-auto-incendiado-y-el-nid07092024/</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/opinion/la-fascinante-experiencia-de-viajar-junto-con-el-papa-nid07092024/</t>
+          <t>https://www.lanacion.com.ar/el-mundo/londres-38-la-historia-que-cruza-a-pinochet-con-un-jerarca-nazi-fugado-a-chile-nid08092024/</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/el-mundo/edmundo-gonzalez-urrutia-se-refugio-durante-mas-de-un-mes-en-la-embajada-de-paises-bajos-en-nid08092024/</t>
+          <t>https://www.lanacion.com.ar/tecnologia/kathleen-booth-la-precursora-de-las-redes-neuronales-que-hace-casi-80-anos-nos-enseno-a-hablar-con-nid08092024/</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/el-mundo/jair-bolsonaro-mostro-su-poder-de-movilizacion-con-una-marcha-multitudinaria-y-pidio-el-juicio-nid07092024/</t>
+          <t>https://www.lanacion.com.ar/conversaciones-de-domingo/dante-sica-el-programa-de-desregulaciones-de-milei-es-similar-al-de-macri-pero-macri-fue-un-liberal-nid08092024/</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/politica/el-inquietante-retorno-de-la-violencia-nid07092024/</t>
+          <t>https://www.lanacion.com.ar/propiedades/inmuebles-comerciales/locales-cuanto-cuesta-alquilar-en-palermo-soho-y-la-avenida-alvear-y-cual-es-la-zona-mas-cara-nid27082024/</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/propiedades/inmuebles-comerciales/locales-cuanto-cuesta-alquilar-en-palermo-soho-y-la-avenida-alvear-y-cual-es-la-zona-mas-cara-nid27082024/</t>
+          <t>https://www.lanacion.com.ar/espectaculos/el-emotivo-festejo-de-cumpleanos-de-paula-chaves-en-compania-de-su-esposo-e-hijos-nid08092024/</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/espectaculos/a-12-anos-de-la-muerte-de-su-hija-blanca-benjamin-vicuna-la-recordo-con-un-emotivo-video-nid08092024/</t>
+          <t>https://www.lanacion.com.ar/espectaculos/personajes/martin-fierro-2024-una-noche-agridulce-con-muchas-estrellas-pero-tambien-con-varias-ausencias-y-un-nid08092024/</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/espectaculos/personajes/martin-fierro-2024-una-noche-agridulce-con-muchas-estrellas-pero-tambien-con-varias-ausencias-y-un-nid08092024/</t>
+          <t>https://www.lanacion.com.ar/espectaculos/anto-roccuzzo-acompano-a-su-hijo-al-entrenamiento-y-quedo-impactada-ante-la-presencia-de-un-animal-nid08092024/</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/espectaculos/anto-roccuzzo-acompano-a-su-hijo-al-entrenamiento-y-quedo-impactada-ante-la-presencia-de-un-animal-nid08092024/</t>
+          <t>https://www.lanacion.com.ar/ideas/el-futuro-del-trabajo-hasta-donde-la-inteligencia-artificial-revolucionara-la-empresa-nid08092024/</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/ideas/el-futuro-del-trabajo-hasta-donde-la-inteligencia-artificial-revolucionara-la-empresa-nid08092024/</t>
+          <t>https://www.lanacion.com.ar/juegos/sopa-de-letras/</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/juegos/sopa-de-letras/</t>
+          <t>https://www.lanacion.com.ar/juegos/trivias/test-de-interes-general-contesta-las-10-preguntas-de-la-semana-sobre-la-avalancha-en-bariloche-la-nid08092024/</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/juegos/trivias/test-de-interes-general-contesta-las-10-preguntas-de-la-semana-sobre-la-avalancha-en-bariloche-la-nid08092024/</t>
+          <t>https://www.lanacion.com.ar/juegos/crucimini/</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/juegos/crucimini/</t>
+          <t>https://www.lanacion.com.ar/juegos/palabra-oculta/</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/juegos/palabra-oculta/</t>
+          <t>https://www.lanacion.com.ar/espectaculos/television/en-la-mesa-de-mirtha-legrand-marta-gonzalez-se-emociono-al-recordar-a-su-amiga-selva-aleman-nid08092024/</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/espectaculos/personajes/el-emotivo-adios-de-mirtha-legrand-a-selva-aleman-era-un-ser-adorable-nid07092024/</t>
+          <t>https://www.lanacion.com.ar/lifestyle/maxima-en-buenos-aires-la-intimidad-de-la-fiesta-de-cumpleanos-80-de-su-madre-en-el-yatch-club-nid06092024/</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/lifestyle/maxima-en-buenos-aires-la-intimidad-de-la-fiesta-de-cumpleanos-80-de-su-madre-en-el-yatch-club-nid06092024/</t>
+          <t>https://www.lanacion.com.ar/espectaculos/franco-colapinto-reacciono-cuando-la-china-suarez-lo-empezo-a-seguir-y-despues-se-arrepintio-nid06092024/</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/espectaculos/franco-colapinto-reacciono-cuando-la-china-suarez-lo-empezo-a-seguir-y-despues-se-arrepintio-nid06092024/</t>
+          <t>https://www.lanacion.com.ar/espectaculos/el-reencuentro-de-wanda-nara-y-mauro-icardi-en-buenos-aires-que-alimento-los-rumores-de-nid08092024/</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/espectaculos/television/los-detalles-del-regreso-de-susana-a-la-tv-grabo-un-sketch-con-caro-pardiaco-y-entrevisto-a-rodrigo-nid07092024/</t>
+          <t>https://www.lanacion.com.ar/sabado/un-clasico-de-la-parrilla-julio-iglesias-mandaba-un-avion-para-hacerse-llevar-los-bifes-a-brasil-nid07092024/</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/sabado/un-clasico-de-la-parrilla-julio-iglesias-mandaba-un-avion-para-hacerse-llevar-los-bifes-a-brasil-nid07092024/</t>
+          <t>https://www.lanacion.com.ar/juegos/trivias/trivia-exclusiva-cuanto-sabes-sobre-la-guerra-de-los-treinta-anos-nid04092024/</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/juegos/trivias/trivia-exclusiva-cuanto-sabes-sobre-la-guerra-de-los-treinta-anos-nid04092024/</t>
+          <t>https://www.lanacion.com.ar/revista-jardin/10-cosas-que-no-sabias-sobre-las-piletas-biologicas-nid08092024/</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/revista-jardin/10-cosas-que-no-sabias-sobre-las-piletas-biologicas-nid08092024/</t>
+          <t>https://www.lanacion.com.ar/economia/negocios/el-local-argentino-que-impuso-las-medialunas-en-una-capital-gastronomica-mundial-nid07092024/</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/economia/negocios/el-local-argentino-que-impuso-las-medialunas-en-una-capital-gastronomica-mundial-nid07092024/</t>
+          <t>https://www.lanacion.com.ar/economia/campo/dia-del-productor-agropecuario-maneja-7300-hectareas-y-cuenta-la-formula-de-un-impactante-logro-en-nid08092024/</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/economia/campo/dia-del-productor-agropecuario-maneja-7300-hectareas-y-cuenta-la-formula-de-un-impactante-logro-en-nid08092024/</t>
+          <t>https://www.lanacion.com.ar/economia/campo/un-lujo-lleno-el-tanque-de-la-camioneta-y-se-quedo-atonico-por-lo-que-tuvo-que-pagar-nid07092024/</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/economia/campo/un-lujo-lleno-el-tanque-de-la-camioneta-y-se-quedo-atonico-por-lo-que-tuvo-que-pagar-nid07092024/</t>
+          <t>https://www.lanacion.com.ar/economia/campo/como-hace-el-hornero-para-construir-su-nido-en-no-mas-de-15-dias-nid07092024/</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/economia/campo/como-hace-el-hornero-para-construir-su-nido-en-no-mas-de-15-dias-nid07092024/</t>
+          <t>https://www.lanacion.com.ar/economia/campo/ramon-diaz-el-refugio-rural-desde-donde-una-de-las-glorias-de-river-planea-otra-vida-y-habla-sin-nid06092024/</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/economia/campo/ramon-diaz-el-refugio-rural-desde-donde-una-de-las-glorias-de-river-planea-otra-vida-y-habla-sin-nid06092024/</t>
+          <t>https://www.lanacion.com.ar/tecnologia/asi-se-veria-campanita-en-la-vida-real-segun-la-inteligencia-artificial-nid06092024/</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/tecnologia/asi-se-veria-campanita-en-la-vida-real-segun-la-inteligencia-artificial-nid06092024/</t>
+          <t>https://www.lanacion.com.ar/tecnologia/las-cinco-carreras-que-nadie-elige-para-estudiar-en-la-argentina-segun-la-inteligencia-artificial-nid06092024/</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/tecnologia/las-cinco-carreras-que-nadie-elige-para-estudiar-en-la-argentina-segun-la-inteligencia-artificial-nid06092024/</t>
+          <t>https://www.lanacion.com.ar/tecnologia/juegos-paralimpicos-de-paris-2024-google-le-dedico-su-doodle-a-la-ceremonia-de-clausura-nid08092024/</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/tecnologia/juegos-paralimpicos-de-paris-2024-google-le-dedico-su-doodle-a-la-ceremonia-de-clausura-nid08092024/</t>
+          <t>https://www.lanacion.com.ar/opinion/milei-mas-rapido-que-kirchner-para-atacar-a-la-prensa-nid08092024/</t>
         </is>
       </c>
     </row>
@@ -938,35 +938,35 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/opinion/llego-el-mes-de-la-alergia-a-la-realidad-nid08092024/</t>
+          <t>https://www.lanacion.com.ar/editoriales/el-desafio-de-construir-un-estado-decente-nid08092024/</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/editoriales/el-desafio-de-construir-un-estado-decente-nid08092024/</t>
+          <t>https://www.lanacion.com.ar/editoriales/juntos-y-arremangados-nid08092024/</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/editoriales/juntos-y-arremangados-nid08092024/</t>
+          <t>https://www.lanacion.com.ar/opinion/llego-el-mes-de-la-alergia-a-la-realidad-nid08092024/</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/opinion/ahora-se-que-no-soy-un-hombre-de-exito-nid08092024/</t>
+          <t>https://www.lanacion.com.ar/horoscopo/horoscopo-las-predicciones-de-jimena-la-torre-para-la-semana-del-8-al-14-de-septiembre-nid08092024/</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/horoscopo/horoscopo-las-predicciones-de-jimena-la-torre-para-la-semana-del-8-al-14-de-septiembre-nid08092024/</t>
+          <t>https://www.lanacion.com.ar/espectaculos/a-12-anos-de-la-muerte-de-su-hija-blanca-benjamin-vicuna-la-recordo-con-un-emotivo-video-nid08092024/</t>
         </is>
       </c>
     </row>
@@ -980,14 +980,14 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/lifestyle/en-las-redes/tras-volverse-viral-en-espana-en-argentina-ya-se-puede-buscar-pareja-en-el-supermercado-cual-es-la-nid07092024/</t>
+          <t>https://www.lanacion.com.ar/lifestyle/mascotas/un-dato-revelador-desmiente-una-creencia-popular-sobre-los-gatos-nid08092024/</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/espectaculos/que-se-sabe-de-la-muerte-de-james-hollcroft-nid08092024/</t>
+          <t>https://www.lanacion.com.ar/lifestyle/cuidado-cuerpo-belleza/agua-con-renacuajos-como-es-la-bebida-con-chia-que-recomiendan-tomar-y-hace-bien-a-la-salud-nid08092024/</t>
         </is>
       </c>
     </row>
@@ -1001,285 +1001,278 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/lifestyle/mascotas/un-dato-revelador-desmiente-una-creencia-popular-sobre-los-gatos-nid08092024/</t>
+          <t>https://www.lanacion.com.ar/lifestyle/cuidado-cuerpo-belleza/cual-es-la-fruta-negra-que-ayuda-a-aumentar-la-masa-muscular-y-previene-el-estrenimiento-nid08092024/</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/lifestyle/cuidado-cuerpo-belleza/agua-con-renacuajos-como-es-la-bebida-con-chia-que-recomiendan-tomar-y-hace-bien-a-la-salud-nid08092024/</t>
+          <t>https://www.lanacion.com.ar/seguridad/una-turista-italiana-denuncio-que-fue-agredida-sexualmente-en-los-esteros-del-ibera-nid08092024/</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/seguridad/una-turista-italiana-denuncio-que-fue-agredida-sexualmente-en-los-esteros-del-ibera-nid08092024/</t>
+          <t>https://www.lanacion.com.ar/deportes/futbol/la-jugada-del-arquero-de-penarol-que-desato-un-escandalo-tres-expulsados-y-seis-amonestados-nid08092024/</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/deportes/futbol/la-jugada-del-arquero-de-penarol-que-desato-un-escandalo-tres-expulsados-y-seis-amonestados-nid08092024/</t>
+          <t>https://www.lanacion.com.ar/espectaculos/anto-roccuzzo-acompano-a-su-hijo-al-entrenamiento-y-quedo-impactada-ante-la-presencia-de-un-animal-nid08092024/</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/el-mundo/el-papa-cumplio-su-promesa-de-visitar-a-misioneros-argentinos-que-trabajan-en-la-periferia-de-la-nid08092024/</t>
+          <t>https://www.lanacion.com.ar/deportes/futbol/lionel-scaloni-sorprendio-con-una-reflexion-acerca-de-su-referente-como-entrenador-nid08092024/</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/deportes/atletismo/el-increible-accidente-de-la-paratleta-italiana-que-perdio-la-medalla-dorada-y-conmovio-a-todos-en-nid08092024/</t>
+          <t>https://www.lanacion.com.ar/espectaculos/personajes/pacho-odonnell-el-edadismo-su-adiccion-a-la-gimnasia-su-regreso-a-los-escenarios-y-por-que-hay-que-nid08092024/</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/deportes/futbol/lionel-scaloni-sorprendio-con-una-reflexion-acerca-de-su-referente-como-entrenador-nid08092024/</t>
+          <t>https://www.lanacion.com.ar/deportes/jugaron-en-grande-el-historico-triunfo-de-los-pumas-frente-a-los-wallabies-en-una-jornada-repleta-de-nid08092024/</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/deportes/jugaron-en-grande-el-historico-triunfo-de-los-pumas-frente-a-los-wallabies-en-una-jornada-repleta-de-nid08092024/</t>
+          <t>https://www.lanacion.com.ar/deportes/polo/polo-los-cambiaso-ya-no-son-dos-sino-tres-pero-camilo-castagnola-pudo-con-todos-y-gano-el-abierto-de-nid08092024/</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/deportes/polo/polo-los-cambiaso-ya-no-son-dos-sino-tres-pero-camilo-castagnola-pudo-con-todos-y-gano-el-abierto-de-nid08092024/</t>
+          <t>https://www.lanacion.com.ar/economia/los-motores-que-aceleran-el-despliegue-de-la-nueva-economia-de-la-introversion-nid08092024/</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/economia/los-motores-que-aceleran-el-despliegue-de-la-nueva-economia-de-la-introversion-nid08092024/</t>
+          <t>https://www.lanacion.com.ar/economia/jubilaciones-que-paso-con-el-poder-adquisitivo-de-los-haberes-en-lo-que-va-de-este-ano-nid02092024/</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/economia/jubilaciones-que-paso-con-el-poder-adquisitivo-de-los-haberes-en-lo-que-va-de-este-ano-nid02092024/</t>
+          <t>https://www.lanacion.com.ar/economia/las-claves-del-blanqueo-segun-las-ultimas-aclaraciones-reglamentarias-nid08092024/</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/economia/las-claves-del-blanqueo-segun-las-ultimas-aclaraciones-reglamentarias-nid08092024/</t>
+          <t>https://www.lanacion.com.ar/economia/finanzas-los-cambios-recientes-en-la-industria-de-fondos-comunes-nid08092024/</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/economia/finanzas-los-cambios-recientes-en-la-industria-de-fondos-comunes-nid08092024/</t>
+          <t>https://www.lanacion.com.ar/espectaculos/cine/asi-cerro-el-festival-de-venecia-de-la-alegria-de-pedro-almodovar-a-la-dolorosa-ausencia-de-nicole-nid07092024/</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/espectaculos/cine/asi-cerro-el-festival-de-venecia-de-la-alegria-de-pedro-almodovar-a-la-dolorosa-ausencia-de-nicole-nid07092024/</t>
+          <t>https://www.lanacion.com.ar/espectaculos/cine/martin-rejtman-entre-las-marcas-de-autor-de-su-cine-el-regreso-de-silvia-prieto-y-el-estreno-de-la-nid07092024/</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/espectaculos/cine/martin-rejtman-entre-las-marcas-de-autor-de-su-cine-el-regreso-de-silvia-prieto-y-el-estreno-de-la-nid07092024/</t>
+          <t>https://www.lanacion.com.ar/espectaculos/television/los-detalles-del-regreso-de-susana-a-la-tv-grabo-un-sketch-con-caro-pardiaco-y-entrevisto-a-rodrigo-nid07092024/</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/espectaculos/television/los-detalles-del-regreso-de-susana-a-la-tv-grabo-un-sketch-con-caro-pardiaco-y-entrevisto-a-rodrigo-nid07092024/</t>
+          <t>https://www.lanacion.com.ar/salud/el-mercado-de-los-sabores-exoticos-y-otros-platos-para-paladares-exigentes-nid07092024/</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/salud/el-mercado-de-los-sabores-exoticos-y-otros-platos-para-paladares-exigentes-nid07092024/</t>
+          <t>https://www.lanacion.com.ar/salud/5-ejercicios-simples-para-aliviar-el-dolor-de-espalda-y-cuello-nid07092024/</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/salud/5-ejercicios-simples-para-aliviar-el-dolor-de-espalda-y-cuello-nid07092024/</t>
+          <t>https://www.lanacion.com.ar/salud/por-que-conectamos-mas-con-las-criticas-que-con-los-elogios-y-repetimos-conductas-nid06092024/</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/salud/por-que-conectamos-mas-con-las-criticas-que-con-los-elogios-y-repetimos-conductas-nid06092024/</t>
+          <t>https://www.lanacion.com.ar/salud/nutricion/oro-blanco-el-probiotico-natural-perfecto-para-aumentar-las-defensas-y-mejorar-el-estado-de-animo-nid03092024/</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/salud/nutricion/oro-blanco-el-probiotico-natural-perfecto-para-aumentar-las-defensas-y-mejorar-el-estado-de-animo-nid03092024/</t>
+          <t>https://www.lanacion.com.ar/autos/cuanto-cuesta-la-ford-ranger-en-septiembre-2024-luego-de-la-baja-del-impuesto-pais-nid06092024/</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/autos/cuanto-cuesta-la-ford-ranger-en-septiembre-2024-luego-de-la-baja-del-impuesto-pais-nid06092024/</t>
+          <t>https://www.lanacion.com.ar/autos/cuanto-cuestan-las-pick-ups-en-septiembre-luego-de-la-baja-de-precios-nid06092024/</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/autos/cuanto-cuestan-las-pick-ups-en-septiembre-luego-de-la-baja-de-precios-nid06092024/</t>
+          <t>https://www.lanacion.com.ar/autos/las-motos-se-suman-a-la-baja-de-precios-cuales-son-los-modelos-que-retrocedieron-en-septiembre-nid04092024/</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/autos/las-motos-se-suman-a-la-baja-de-precios-cuales-son-los-modelos-que-retrocedieron-en-septiembre-nid04092024/</t>
+          <t>https://www.lanacion.com.ar/autos/cuanto-cuesta-el-toyota-corolla-cross-en-septiembre-2024-luego-de-la-baja-del-impuesto-pais-nid06092024/</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/autos/cuanto-cuesta-el-toyota-corolla-cross-en-septiembre-2024-luego-de-la-baja-del-impuesto-pais-nid06092024/</t>
+          <t>https://www.lanacion.com.ar/propiedades/casas-y-departamentos/historias-es-argentino-compro-un-burdel-para-crear-un-corredor-en-zona-norte-y-hara-un-cable-carril-nid07092024/</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/propiedades/casas-y-departamentos/historias-es-argentino-compro-un-burdel-para-crear-un-corredor-en-zona-norte-y-hara-un-cable-carril-nid07092024/</t>
+          <t>https://www.lanacion.com.ar/propiedades/casas-y-departamentos/el-barrio-verde-que-vive-un-boom-de-construccion-y-tiene-hasta-dos-proyectos-en-una-misma-cuadra-nid02092024/</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/propiedades/casas-y-departamentos/el-barrio-verde-que-vive-un-boom-de-construccion-y-tiene-hasta-dos-proyectos-en-una-misma-cuadra-nid02092024/</t>
+          <t>https://www.lanacion.com.ar/propiedades/construccion-y-diseno/historias-es-argentino-se-anticipo-a-un-megaproyecto-petrolero-y-desarrollo-la-ciudad-que-potenciara-nid06092024/</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/propiedades/construccion-y-diseno/historias-es-argentino-se-anticipo-a-un-megaproyecto-petrolero-y-desarrollo-la-ciudad-que-potenciara-nid06092024/</t>
+          <t>https://www.lanacion.com.ar/propiedades/casas-y-departamentos/la-ciudad-de-nueva-york-que-paga-us9000-por-mudarse-cuales-son-los-requisitos-nid06092024/</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/propiedades/casas-y-departamentos/la-ciudad-de-nueva-york-que-paga-us9000-por-mudarse-cuales-son-los-requisitos-nid06092024/</t>
+          <t>https://www.lanacion.com.ar/economia/campo/estupor-frente-a-un-grave-atentado-y-los-avances-de-la-desregulacion-nid07092024/</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/economia/campo/estupor-frente-a-un-grave-atentado-y-los-avances-de-la-desregulacion-nid07092024/</t>
+          <t>https://www.lanacion.com.ar/economia/campo/agricultura/el-repunte-del-maiz-y-de-la-soja-en-chicago-se-mira-pero-no-se-copia-en-el-mercado-argentino-nid07092024/</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/economia/campo/agricultura/el-repunte-del-maiz-y-de-la-soja-en-chicago-se-mira-pero-no-se-copia-en-el-mercado-argentino-nid07092024/</t>
+          <t>https://www.lanacion.com.ar/economia/campo/mas-papistas-que-el-papa-fuerte-malestar-entre-productores-por-una-marcha-atras-del-gobierno-con-una-nid06092024/</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/economia/campo/mas-papistas-que-el-papa-fuerte-malestar-entre-productores-por-una-marcha-atras-del-gobierno-con-una-nid06092024/</t>
+          <t>https://www.lanacion.com.ar/economia/campo/no-nos-van-a-callar-el-presidente-de-la-rural-califico-al-atentado-de-un-episodio-de-una-argentina-nid06092024/</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/economia/campo/no-nos-van-a-callar-el-presidente-de-la-rural-califico-al-atentado-de-un-episodio-de-una-argentina-nid06092024/</t>
+          <t>https://www.lanacion.com.ar/lifestyle/controlaba-las-piletas-de-un-completo-cuando-noto-algo-extrano-que-flotaba-estaba-helada-e-inmovil-nid08092024/</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/lifestyle/controlaba-las-piletas-de-un-completo-cuando-noto-algo-extrano-que-flotaba-estaba-helada-e-inmovil-nid08092024/</t>
+          <t>https://www.lanacion.com.ar/sabado/un-clasico-de-la-parrilla-julio-iglesias-mandaba-un-avion-para-hacerse-llevar-los-bifes-a-brasil-nid07092024/</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/sabado/un-clasico-de-la-parrilla-julio-iglesias-mandaba-un-avion-para-hacerse-llevar-los-bifes-a-brasil-nid07092024/</t>
+          <t>https://www.lanacion.com.ar/lifestyle/que-es-la-gente-nutritiva-y-cuales-son-sus-caracteristicas-nid17112023/</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/lifestyle/que-es-la-gente-nutritiva-y-cuales-son-sus-caracteristicas-nid17112023/</t>
+          <t>https://www.lanacion.com.ar/revista-lugares/la-ruta-de-los-abstemios-planes-entre-las-bodegas-mendocinas-sin-tomar-vino-nid07092024/</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/revista-lugares/la-ruta-de-los-abstemios-planes-entre-las-bodegas-mendocinas-sin-tomar-vino-nid07092024/</t>
+          <t>https://www.lanacion.com.ar/revista-living/10-ideas-para-ponerle-onda-a-tu-sofa-nid04092024/</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/revista-living/10-ideas-para-ponerle-onda-a-tu-sofa-nid04092024/</t>
+          <t>https://www.lanacion.com.ar/sociedad/natividad-de-la-santisima-virgen-maria-su-historia-y-que-oracion-rezar-para-pedir-su-ayuda-nid08092024/</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/sociedad/natividad-de-la-santisima-virgen-maria-su-historia-y-que-oracion-rezar-para-pedir-su-ayuda-nid08092024/</t>
+          <t>https://www.lanacion.com.ar/feriados/2024/11-de-septiembre-el-dia-del-maestro-es-feriado-nid08092024/</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/feriados/2024/11-de-septiembre-el-dia-del-maestro-es-feriado-nid08092024/</t>
+          <t>https://www.lanacion.com.ar/economia/jubilados-anses-fijo-el-haber-maximo-a-partir-de-septiembre-en-cuanto-queda-nid08092024/</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
-        <is>
-          <t>https://www.lanacion.com.ar/economia/jubilados-anses-fijo-el-haber-maximo-a-partir-de-septiembre-en-cuanto-queda-nid08092024/</t>
-        </is>
-      </c>
-    </row>
-    <row r="122">
-      <c r="A122" t="inlineStr">
         <is>
           <t>https://www.lanacion.com.ar/loterias/quini-6-cual-es-el-premio-para-el-sorteo-de-este-domingo-8-de-septiembre-nid08092024/</t>
         </is>

</xml_diff>